<commit_message>
Started the bill of materials (BOM), proper. So far it has only the parts I didn't already have in stock.
</commit_message>
<xml_diff>
--- a/hardware/gMeter-bom.xlsx
+++ b/hardware/gMeter-bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="3980" windowWidth="20860" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="28080" yWindow="6760" windowWidth="20860" windowHeight="16340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,80 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Element14</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ref</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>X1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+  <si>
+    <t>Yellow</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TO BE COMPLETED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nz.element14.com 'next day delivery' cheapest pricing BOM</t>
+  </si>
+  <si>
+    <t>nz.element14.com</t>
+  </si>
+  <si>
+    <t>ele14 Part No.</t>
+  </si>
+  <si>
+    <t>Price Ea.</t>
+  </si>
+  <si>
+    <t>MOQ</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>gMeter v1.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>as at 2013-06-12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SM1206</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kingbright</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>KP-3216EC</t>
+  </si>
+  <si>
+    <t>LED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>KP-3216SEC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SM1206</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kingbright</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>KP-3216YC</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -37,35 +100,51 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>12.0MHz</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKU</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Case</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>5x3.2mm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>12MHz</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABM3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abracon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABM3-12.000MHZ-D2Y-T</t>
+  </si>
+  <si>
+    <t>KP-3216SGC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Green</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Orange</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manufacturer Name</t>
+  </si>
+  <si>
+    <t>Mfr Part No.</t>
+  </si>
+  <si>
+    <t>Qty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -85,20 +164,136 @@
       <color indexed="12"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="62"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="18"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -110,7 +305,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -118,13 +313,76 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -455,66 +713,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="B4:F8"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="5" max="5" width="10.7109375" style="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6">
-      <c r="B4" t="s">
+    <row r="1" spans="1:10" ht="23">
+      <c r="A1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" ht="16">
+      <c r="A2" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="18">
+      <c r="A4" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="11">
+        <v>8530025</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="C7" s="13">
+        <v>10</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="25">
+        <v>8530009</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="C8" s="13">
+        <v>10</v>
+      </c>
+      <c r="D8" s="20">
+        <v>2</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="25">
+        <v>8530041</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="C9" s="13">
+        <v>10</v>
+      </c>
+      <c r="D9" s="20">
+        <v>3</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="3" t="s">
+      <c r="J9" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="25">
+        <v>8530033</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0.254</v>
+      </c>
+      <c r="C10" s="13">
+        <v>10</v>
+      </c>
+      <c r="D10" s="20">
+        <v>2</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2">
+        <v>2101327</v>
+      </c>
+      <c r="B11" s="21">
+        <v>2.88</v>
+      </c>
+      <c r="C11" s="13">
         <v>1</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="2">
-        <v>2101327</v>
-      </c>
-    </row>
+      <c r="D11" s="20">
+        <v>1</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="20"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="20"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" ht="16"/>
+    <row r="18" ht="16"/>
+    <row r="19" ht="16"/>
+    <row r="20" ht="16"/>
+    <row r="21" ht="16"/>
+    <row r="22" ht="16"/>
+    <row r="23" ht="16"/>
+    <row r="24" ht="16"/>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:F4"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" display="http://nz.element14.com/abracon/abm3-12-000mhz-d2-t/crystal-12mhz-18pf-smd/dp/2101327"/>
+    <hyperlink ref="A7" r:id="rId1" display="http://nz.element14.com/kingbright/kp-3216ec/led-1206-red-230mcd-630nm/dp/8530025"/>
+    <hyperlink ref="A8" r:id="rId2" display="http://nz.element14.com/kingbright/kp-3216sec/led-smd-1206-orange/dp/8530009"/>
+    <hyperlink ref="A9" r:id="rId3" display="http://nz.element14.com/kingbright/kp-3216yc/led-smd-1206-yellow/dp/8530041"/>
+    <hyperlink ref="A11" r:id="rId4" display="http://nz.element14.com/abracon/abm3-12-000mhz-d2-t/crystal-12mhz-18pf-smd/dp/2101327"/>
+    <hyperlink ref="A10" r:id="rId5" display="http://nz.element14.com/kingbright/kp-3216sgc/led-1206-green-12mcd-565nm/dp/8530033"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Minor update to bill of materials (BOM)
</commit_message>
<xml_diff>
--- a/hardware/gMeter-bom.xlsx
+++ b/hardware/gMeter-bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28080" yWindow="6760" windowWidth="20860" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="17420" yWindow="6960" windowWidth="20860" windowHeight="16340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Yellow</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -32,9 +32,6 @@
     <t>nz.element14.com 'next day delivery' cheapest pricing BOM</t>
   </si>
   <si>
-    <t>nz.element14.com</t>
-  </si>
-  <si>
     <t>ele14 Part No.</t>
   </si>
   <si>
@@ -138,6 +135,34 @@
   </si>
   <si>
     <t>Qty</t>
+  </si>
+  <si>
+    <t>Atmel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATMEGA88PA-MU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATmega88P MLF-32</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>32MLF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>20MHz</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MLF Version</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prices are NZD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -184,12 +209,6 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b/>
       <u/>
       <sz val="10"/>
       <color indexed="8"/>
@@ -203,6 +222,12 @@
     <font>
       <sz val="10"/>
       <color indexed="18"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -305,14 +330,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -325,22 +347,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -367,7 +386,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -380,8 +399,29 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -713,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -724,304 +764,397 @@
     <col min="2" max="2" width="7.85546875" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.140625" customWidth="1"/>
     <col min="7" max="7" width="1.42578125" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="16">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="9">
+        <v>8530025</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="C6" s="11">
+        <v>10</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" ht="18">
-      <c r="A4" s="26" t="s">
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="20">
+        <v>8530009</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="C7" s="11">
+        <v>10</v>
+      </c>
+      <c r="D7" s="18">
+        <v>2</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="20">
+        <v>8530041</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="C8" s="11">
+        <v>10</v>
+      </c>
+      <c r="D8" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="E8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="20">
+        <v>8530033</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0.254</v>
+      </c>
+      <c r="C9" s="11">
+        <v>10</v>
+      </c>
+      <c r="D9" s="18">
+        <v>2</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="19"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="2"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="27"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="27"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="20">
+        <v>1715491</v>
+      </c>
+      <c r="B15" s="19">
+        <v>4.49</v>
+      </c>
+      <c r="C15" s="11">
+        <v>1</v>
+      </c>
+      <c r="D15" s="18">
+        <v>1</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="11">
-        <v>8530025</v>
-      </c>
-      <c r="B7" s="12">
-        <v>0.23599999999999999</v>
-      </c>
-      <c r="C7" s="13">
-        <v>10</v>
-      </c>
-      <c r="D7" s="14">
+      <c r="F15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="29">
+        <v>2101327</v>
+      </c>
+      <c r="B16" s="19">
+        <v>2.88</v>
+      </c>
+      <c r="C16" s="11">
         <v>1</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="22">
-        <v>8530009</v>
-      </c>
-      <c r="B8" s="12">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="C8" s="13">
-        <v>10</v>
-      </c>
-      <c r="D8" s="20">
-        <v>2</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="22">
-        <v>8530041</v>
-      </c>
-      <c r="B9" s="12">
-        <v>0.23599999999999999</v>
-      </c>
-      <c r="C9" s="13">
-        <v>10</v>
-      </c>
-      <c r="D9" s="20">
-        <v>3</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="16" t="s">
+      <c r="D16" s="18">
+        <v>1</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="22">
-        <v>8530033</v>
-      </c>
-      <c r="B10" s="12">
-        <v>0.254</v>
-      </c>
-      <c r="C10" s="13">
-        <v>10</v>
-      </c>
-      <c r="D10" s="20">
-        <v>2</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="2">
-        <v>2101327</v>
-      </c>
-      <c r="B11" s="21">
-        <v>2.88</v>
-      </c>
-      <c r="C11" s="13">
+      <c r="I16" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="20">
-        <v>1</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="3"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="3"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="23" t="s">
-        <v>1</v>
-      </c>
-    </row>
+    </row>
+    <row r="21" spans="1:10" ht="16"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:G1"/>
+  <mergeCells count="2">
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" display="http://nz.element14.com/kingbright/kp-3216ec/led-1206-red-230mcd-630nm/dp/8530025"/>
-    <hyperlink ref="A8" r:id="rId2" display="http://nz.element14.com/kingbright/kp-3216sec/led-smd-1206-orange/dp/8530009"/>
-    <hyperlink ref="A9" r:id="rId3" display="http://nz.element14.com/kingbright/kp-3216yc/led-smd-1206-yellow/dp/8530041"/>
-    <hyperlink ref="A11" r:id="rId4" display="http://nz.element14.com/abracon/abm3-12-000mhz-d2-t/crystal-12mhz-18pf-smd/dp/2101327"/>
-    <hyperlink ref="A10" r:id="rId5" display="http://nz.element14.com/kingbright/kp-3216sgc/led-1206-green-12mcd-565nm/dp/8530033"/>
+    <hyperlink ref="A6" r:id="rId1" display="http://nz.element14.com/kingbright/kp-3216ec/led-1206-red-230mcd-630nm/dp/8530025"/>
+    <hyperlink ref="A7" r:id="rId2" display="http://nz.element14.com/kingbright/kp-3216sec/led-smd-1206-orange/dp/8530009"/>
+    <hyperlink ref="A8" r:id="rId3" display="http://nz.element14.com/kingbright/kp-3216yc/led-smd-1206-yellow/dp/8530041"/>
+    <hyperlink ref="A9" r:id="rId4" display="http://nz.element14.com/kingbright/kp-3216sgc/led-1206-green-12mcd-565nm/dp/8530033"/>
+    <hyperlink ref="A16" r:id="rId5" display="http://nz.element14.com/abracon/abm3-12-000mhz-d2-t/crystal-12mhz-18pf-smd/dp/2101327"/>
+    <hyperlink ref="A15" r:id="rId6" display="http://nz.element14.com/atmel/atmega88pa-mu/ic-mcu-8bit-avr-8k-flash-32mlf/dp/1715491?Ntt=1715491"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>